<commit_message>
ECP-1152: fixes forecast creation process; adds integ test
</commit_message>
<xml_diff>
--- a/estatioapp/app/src/test/java/org/estatio/module/capex/integtests/project/ForecastITPR001.xlsx
+++ b/estatioapp/app/src/test/java/org/estatio/module/capex/integtests/project/ForecastITPR001.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/johan/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/johan/src/estatio-ecp/estatio/estatioapp/app/src/test/java/org/estatio/module/capex/integtests/project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58B8186F-4A8D-B847-93A9-8256D0502EB6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED81E5F6-0562-414D-A5F8-6EBBDCA58543}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="35840" windowHeight="21940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -444,7 +444,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H8" sqref="H8"/>
+      <selection pane="bottomLeft" activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -527,8 +527,8 @@
         <v>0</v>
       </c>
       <c r="N2" s="4">
-        <f>SUM(E2:H2)</f>
-        <v>60000</v>
+        <f>SUM(F2:H2)</f>
+        <v>50000</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.2">
@@ -563,7 +563,7 @@
         <v>0</v>
       </c>
       <c r="N3" s="4">
-        <f>SUM(E3:H3)</f>
+        <f t="shared" ref="N3:N7" si="0">SUM(E3:H3)</f>
         <v>9000</v>
       </c>
     </row>
@@ -599,12 +599,12 @@
         <v>0</v>
       </c>
       <c r="N4" s="4">
-        <f>SUM(E4:H4)</f>
+        <f t="shared" si="0"/>
         <v>55000</v>
       </c>
       <c r="O4" s="4">
         <f>SUM(N2:N4)</f>
-        <v>124000</v>
+        <v>114000</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.2">
@@ -620,9 +620,6 @@
       <c r="D5" s="1">
         <v>2020</v>
       </c>
-      <c r="E5" s="3">
-        <v>1000000</v>
-      </c>
       <c r="F5" s="3">
         <v>500000</v>
       </c>
@@ -639,8 +636,8 @@
         <v>0</v>
       </c>
       <c r="N5" s="4">
-        <f>SUM(E5:H5)</f>
-        <v>5250000</v>
+        <f>SUM(F5:H5)</f>
+        <v>4250000</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.2">
@@ -675,7 +672,7 @@
         <v>0</v>
       </c>
       <c r="N6" s="4">
-        <f>SUM(E6:H6)</f>
+        <f t="shared" si="0"/>
         <v>2200000</v>
       </c>
     </row>
@@ -699,7 +696,7 @@
         <v>1200000</v>
       </c>
       <c r="G7" s="3">
-        <v>0</v>
+        <v>1026600</v>
       </c>
       <c r="H7" s="3">
         <v>300000</v>
@@ -711,12 +708,12 @@
         <v>0</v>
       </c>
       <c r="N7" s="4">
-        <f>SUM(E7:H7)</f>
-        <v>2400000</v>
+        <f t="shared" si="0"/>
+        <v>3426600</v>
       </c>
       <c r="O7" s="4">
         <f>SUM(N5:N7)</f>
-        <v>9850000</v>
+        <v>9876600</v>
       </c>
     </row>
   </sheetData>

</xml_diff>